<commit_message>
feature names with labels
</commit_message>
<xml_diff>
--- a/ADHD_CC200_ROI_labels.xlsx
+++ b/ADHD_CC200_ROI_labels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yagmu\Desktop\Auburn\Research\project\Logistic regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yagmu\Box\Auburn\Research\project\Logistic regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512502E6-236B-49A8-B402-6348DDA6E2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DD051F-DD3E-4170-99AE-3330676A6B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="286">
   <si>
     <t>Superior Frontal Gyrus          Frontal_Sup_Orb_R</t>
   </si>
@@ -893,75 +893,6 @@
   </si>
   <si>
     <t>cc200 value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected </t>
-  </si>
-  <si>
-    <t>names</t>
-  </si>
-  <si>
-    <t>freq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insula_R' </t>
-  </si>
-  <si>
-    <t>names2</t>
-  </si>
-  <si>
-    <t>114,40</t>
-  </si>
-  <si>
-    <t>lobe name</t>
-  </si>
-  <si>
-    <t>frequency</t>
-  </si>
-  <si>
-    <t>Insula</t>
-  </si>
-  <si>
-    <t>Frontal</t>
-  </si>
-  <si>
-    <t>Temporal</t>
-  </si>
-  <si>
-    <t>Supp_motor</t>
-  </si>
-  <si>
-    <t>Vermis</t>
-  </si>
-  <si>
-    <t>Occipital</t>
-  </si>
-  <si>
-    <t>Cingulum</t>
-  </si>
-  <si>
-    <t>Paracentral</t>
-  </si>
-  <si>
-    <t>Lingual</t>
-  </si>
-  <si>
-    <t>Supramarginal</t>
-  </si>
-  <si>
-    <t>Pallidum</t>
-  </si>
-  <si>
-    <t>Cerebelum</t>
-  </si>
-  <si>
-    <t>Caudate</t>
-  </si>
-  <si>
-    <t>Precuneus</t>
-  </si>
-  <si>
-    <t>selected by lasso</t>
   </si>
 </sst>
 </file>
@@ -992,21 +923,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor theme="0" tint="-0.14999847407452621"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1014,26 +939,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1054,24 +964,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <font>
         <b val="0"/>
@@ -1106,43 +1003,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1203,54 +1063,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="B2:K192" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="B2:K192" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Channel's region" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="x-coordinate" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="y-coordinate" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="z-coordinate" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Channel region (again)" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="cc200 value" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{E974CCF6-1423-4228-AF93-8D7731AA3E73}" name="selected " dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{3FD20BFC-DC2F-4C2E-923D-3C60612D8E1A}" name="names" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{83DD14A8-A1CF-4550-922B-413B6AA5334C}" name="names2" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{EA9A067B-8D71-4097-99BD-361E95AD6C42}" name="freq" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="B2:G192" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="B2:G192" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Channel's region" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="x-coordinate" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="y-coordinate" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="z-coordinate" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Channel region (again)" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="cc200 value" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A2:A192" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A2:A192" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="A2:A192" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Channel no." dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Channel no." dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5D850A01-21E3-457B-8A6D-028E0818C66D}" name="Table4" displayName="Table4" ref="M2:N17" totalsRowShown="0">
-  <autoFilter ref="M2:N17" xr:uid="{5D850A01-21E3-457B-8A6D-028E0818C66D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M3:N17">
-    <sortCondition descending="1" ref="N2:N17"/>
-  </sortState>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{62CF746A-A953-4248-9795-6A6FF65B9EAD}" name="lobe name"/>
-    <tableColumn id="2" xr3:uid="{9FB57489-797B-4CA2-946B-859209EA5CDA}" name="frequency" dataDxfId="0">
-      <calculatedColumnFormula>10*381</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1288,9 +1128,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1323,26 +1163,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1375,26 +1198,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1571,10 +1377,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q192"/>
+  <dimension ref="A2:G192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1585,19 +1391,9 @@
     <col min="5" max="5" width="15.90625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="22.7265625" style="6" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1796875" customWidth="1"/>
-    <col min="16" max="16" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="P1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>284</v>
       </c>
@@ -1619,26 +1415,8 @@
       <c r="G2" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="M2" t="s">
-        <v>292</v>
-      </c>
-      <c r="N2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1660,32 +1438,8 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="2">
-        <v>54.21</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="K3" s="2">
-        <v>381</v>
-      </c>
-      <c r="M3" t="s">
-        <v>295</v>
-      </c>
-      <c r="N3">
-        <v>2903</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q3" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1707,32 +1461,8 @@
       <c r="G4" s="1">
         <v>3</v>
       </c>
-      <c r="H4" s="2">
-        <v>72.680000000000007</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="K4" s="2">
-        <v>381</v>
-      </c>
-      <c r="M4" t="s">
-        <v>296</v>
-      </c>
-      <c r="N4">
-        <v>1179</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1754,32 +1484,8 @@
       <c r="G5" s="1">
         <v>4</v>
       </c>
-      <c r="H5" s="2">
-        <v>101.85</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="K5" s="2">
-        <v>381</v>
-      </c>
-      <c r="M5" t="s">
-        <v>294</v>
-      </c>
-      <c r="N5">
-        <v>762</v>
-      </c>
-      <c r="P5" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q5" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1801,32 +1507,8 @@
       <c r="G6" s="1">
         <v>6</v>
       </c>
-      <c r="H6" s="2">
-        <v>116.89</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="K6" s="2">
-        <v>381</v>
-      </c>
-      <c r="M6" t="s">
-        <v>298</v>
-      </c>
-      <c r="N6">
-        <v>688</v>
-      </c>
-      <c r="P6" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q6" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1848,32 +1530,8 @@
       <c r="G7" s="1">
         <v>7</v>
       </c>
-      <c r="H7" s="2">
-        <v>104.34</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="K7" s="2">
-        <v>377</v>
-      </c>
-      <c r="M7" t="s">
-        <v>301</v>
-      </c>
-      <c r="N7">
-        <v>639</v>
-      </c>
-      <c r="P7" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1895,32 +1553,8 @@
       <c r="G8" s="1">
         <v>8</v>
       </c>
-      <c r="H8" s="2">
-        <v>151.14699999999999</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="K8" s="2">
-        <v>377</v>
-      </c>
-      <c r="M8" t="s">
-        <v>300</v>
-      </c>
-      <c r="N8">
-        <v>542</v>
-      </c>
-      <c r="P8" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q8" s="9" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1942,32 +1576,8 @@
       <c r="G9" s="1">
         <v>9</v>
       </c>
-      <c r="H9" s="2">
-        <v>72.11</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="K9" s="2">
-        <v>363</v>
-      </c>
-      <c r="M9" t="s">
-        <v>302</v>
-      </c>
-      <c r="N9">
-        <v>381</v>
-      </c>
-      <c r="P9" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q9" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1989,32 +1599,8 @@
       <c r="G10" s="1">
         <v>10</v>
       </c>
-      <c r="H10" s="2">
-        <v>150.114</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="K10" s="2">
-        <v>363</v>
-      </c>
-      <c r="M10" t="s">
-        <v>297</v>
-      </c>
-      <c r="N10">
-        <v>377</v>
-      </c>
-      <c r="P10" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q10" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -2036,32 +1622,8 @@
       <c r="G11" s="1">
         <v>12</v>
       </c>
-      <c r="H11" s="2">
-        <v>126.2</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="K11" s="2">
-        <v>325</v>
-      </c>
-      <c r="M11" t="s">
-        <v>303</v>
-      </c>
-      <c r="N11">
-        <v>377</v>
-      </c>
-      <c r="P11" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q11" s="9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -2083,32 +1645,8 @@
       <c r="G12" s="1">
         <v>13</v>
       </c>
-      <c r="H12" s="2">
-        <v>124.99</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="K12" s="2">
-        <v>284</v>
-      </c>
-      <c r="M12" t="s">
-        <v>127</v>
-      </c>
-      <c r="N12">
-        <v>363</v>
-      </c>
-      <c r="P12" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q12" s="10" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2130,32 +1668,8 @@
       <c r="G13" s="1">
         <v>14</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K13" s="2">
-        <v>281</v>
-      </c>
-      <c r="M13" t="s">
-        <v>304</v>
-      </c>
-      <c r="N13">
-        <v>281</v>
-      </c>
-      <c r="P13" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q13" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2177,32 +1691,8 @@
       <c r="G14" s="1">
         <v>15</v>
       </c>
-      <c r="H14" s="2">
-        <v>162.72999999999999</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="K14" s="2">
-        <v>267</v>
-      </c>
-      <c r="M14" t="s">
-        <v>299</v>
-      </c>
-      <c r="N14">
-        <v>267</v>
-      </c>
-      <c r="P14" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q14" s="9" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2224,32 +1714,8 @@
       <c r="G15" s="1">
         <v>16</v>
       </c>
-      <c r="H15" s="2">
-        <v>47.21</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="K15" s="2">
-        <v>258</v>
-      </c>
-      <c r="M15" t="s">
-        <v>305</v>
-      </c>
-      <c r="N15">
-        <v>267</v>
-      </c>
-      <c r="P15" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q15" s="10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2271,32 +1737,8 @@
       <c r="G16" s="1">
         <v>17</v>
       </c>
-      <c r="H16" s="2">
-        <v>146.88999999999999</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="K16" s="2">
-        <v>235</v>
-      </c>
-      <c r="M16" t="s">
-        <v>306</v>
-      </c>
-      <c r="N16">
-        <v>207</v>
-      </c>
-      <c r="P16" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q16" s="9" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2318,32 +1760,8 @@
       <c r="G17" s="1">
         <v>18</v>
       </c>
-      <c r="H17" s="2">
-        <v>108.27</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="K17" s="2">
-        <v>207</v>
-      </c>
-      <c r="M17" t="s">
-        <v>307</v>
-      </c>
-      <c r="N17">
-        <v>149</v>
-      </c>
-      <c r="P17" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q17" s="9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2365,26 +1783,8 @@
       <c r="G18" s="1">
         <v>19</v>
       </c>
-      <c r="H18" s="2">
-        <v>108.91</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="K18" s="2">
-        <v>201</v>
-      </c>
-      <c r="P18" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q18" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -2406,26 +1806,8 @@
       <c r="G19" s="1">
         <v>20</v>
       </c>
-      <c r="H19" s="2">
-        <v>114.28</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="K19" s="2">
-        <v>172</v>
-      </c>
-      <c r="P19" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q19" s="10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -2447,26 +1829,8 @@
       <c r="G20" s="1">
         <v>21</v>
       </c>
-      <c r="H20" s="2">
-        <v>173.9</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="K20" s="2">
-        <v>149</v>
-      </c>
-      <c r="P20" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q20" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -2488,18 +1852,8 @@
       <c r="G21" s="1">
         <v>22</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="P21" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q21" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -2521,18 +1875,8 @@
       <c r="G22" s="1">
         <v>23</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="P22" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q22" s="9" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -2554,18 +1898,8 @@
       <c r="G23" s="1">
         <v>24</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="P23" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q23" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -2587,18 +1921,8 @@
       <c r="G24" s="1">
         <v>26</v>
       </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="P24" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q24" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2620,18 +1944,8 @@
       <c r="G25" s="1">
         <v>27</v>
       </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="P25" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q25" s="10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -2653,18 +1967,8 @@
       <c r="G26" s="1">
         <v>28</v>
       </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="P26" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q26" s="10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -2686,18 +1990,8 @@
       <c r="G27" s="1">
         <v>29</v>
       </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="P27" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q27" s="10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -2719,18 +2013,8 @@
       <c r="G28" s="1">
         <v>30</v>
       </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="P28" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q28" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -2752,18 +2036,8 @@
       <c r="G29" s="1">
         <v>31</v>
       </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="P29" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q29" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -2785,18 +2059,8 @@
       <c r="G30" s="1">
         <v>32</v>
       </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="P30" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q30" s="10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -2818,18 +2082,8 @@
       <c r="G31" s="1">
         <v>33</v>
       </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="P31" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q31" s="9" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -2851,18 +2105,8 @@
       <c r="G32" s="1">
         <v>35</v>
       </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="P32" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q32" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -2884,18 +2128,8 @@
       <c r="G33" s="1">
         <v>36</v>
       </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="P33" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q33" s="9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -2917,18 +2151,8 @@
       <c r="G34" s="1">
         <v>37</v>
       </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="P34" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q34" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -2950,18 +2174,8 @@
       <c r="G35" s="1">
         <v>38</v>
       </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="P35" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q35" s="9" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -2983,18 +2197,8 @@
       <c r="G36" s="1">
         <v>39</v>
       </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="P36" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q36" s="9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -3016,18 +2220,8 @@
       <c r="G37" s="1">
         <v>40</v>
       </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="P37" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q37" s="10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -3049,18 +2243,8 @@
       <c r="G38" s="1">
         <v>41</v>
       </c>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="P38" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q38" s="9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -3082,18 +2266,8 @@
       <c r="G39" s="1">
         <v>42</v>
       </c>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="P39" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q39" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -3115,18 +2289,8 @@
       <c r="G40" s="1">
         <v>43</v>
       </c>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="P40" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q40" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -3148,18 +2312,8 @@
       <c r="G41" s="1">
         <v>44</v>
       </c>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="P41" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q41" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>40</v>
       </c>
@@ -3181,18 +2335,8 @@
       <c r="G42" s="1">
         <v>45</v>
       </c>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="P42" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q42" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -3214,18 +2358,8 @@
       <c r="G43" s="1">
         <v>46</v>
       </c>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="P43" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q43" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -3247,18 +2381,8 @@
       <c r="G44" s="1">
         <v>47</v>
       </c>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="P44" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q44" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>43</v>
       </c>
@@ -3280,18 +2404,8 @@
       <c r="G45" s="1">
         <v>48</v>
       </c>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="P45" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q45" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>44</v>
       </c>
@@ -3313,18 +2427,8 @@
       <c r="G46" s="1">
         <v>49</v>
       </c>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="P46" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q46" s="10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>45</v>
       </c>
@@ -3346,18 +2450,8 @@
       <c r="G47" s="1">
         <v>50</v>
       </c>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="P47" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q47" s="9" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -3379,15 +2473,8 @@
       <c r="G48" s="1">
         <v>51</v>
       </c>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-      <c r="O48" s="11">
-        <v>112110</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>47</v>
       </c>
@@ -3409,12 +2496,8 @@
       <c r="G49" s="1">
         <v>52</v>
       </c>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-    </row>
-    <row r="50" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>48</v>
       </c>
@@ -3436,12 +2519,8 @@
       <c r="G50" s="1">
         <v>53</v>
       </c>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-    </row>
-    <row r="51" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>49</v>
       </c>
@@ -3463,12 +2542,8 @@
       <c r="G51" s="1">
         <v>54</v>
       </c>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-    </row>
-    <row r="52" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>50</v>
       </c>
@@ -3490,12 +2565,8 @@
       <c r="G52" s="1">
         <v>55</v>
       </c>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-    </row>
-    <row r="53" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>51</v>
       </c>
@@ -3517,12 +2588,8 @@
       <c r="G53" s="1">
         <v>56</v>
       </c>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-    </row>
-    <row r="54" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>52</v>
       </c>
@@ -3544,12 +2611,8 @@
       <c r="G54" s="1">
         <v>57</v>
       </c>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-    </row>
-    <row r="55" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>53</v>
       </c>
@@ -3571,12 +2634,8 @@
       <c r="G55" s="1">
         <v>58</v>
       </c>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-    </row>
-    <row r="56" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>54</v>
       </c>
@@ -3598,12 +2657,8 @@
       <c r="G56" s="1">
         <v>59</v>
       </c>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-    </row>
-    <row r="57" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>55</v>
       </c>
@@ -3625,12 +2680,8 @@
       <c r="G57" s="1">
         <v>60</v>
       </c>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
-    </row>
-    <row r="58" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>56</v>
       </c>
@@ -3652,12 +2703,8 @@
       <c r="G58" s="1">
         <v>61</v>
       </c>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
-    </row>
-    <row r="59" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>57</v>
       </c>
@@ -3679,12 +2726,8 @@
       <c r="G59" s="1">
         <v>62</v>
       </c>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-    </row>
-    <row r="60" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>58</v>
       </c>
@@ -3706,12 +2749,8 @@
       <c r="G60" s="1">
         <v>63</v>
       </c>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-    </row>
-    <row r="61" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>59</v>
       </c>
@@ -3733,12 +2772,8 @@
       <c r="G61" s="1">
         <v>64</v>
       </c>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-    </row>
-    <row r="62" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>60</v>
       </c>
@@ -3760,12 +2795,8 @@
       <c r="G62" s="1">
         <v>65</v>
       </c>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-    </row>
-    <row r="63" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>61</v>
       </c>
@@ -3787,12 +2818,8 @@
       <c r="G63" s="1">
         <v>66</v>
       </c>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
-    </row>
-    <row r="64" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>62</v>
       </c>
@@ -3814,12 +2841,8 @@
       <c r="G64" s="1">
         <v>67</v>
       </c>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-    </row>
-    <row r="65" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>63</v>
       </c>
@@ -3841,12 +2864,8 @@
       <c r="G65" s="1">
         <v>69</v>
       </c>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
-    </row>
-    <row r="66" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>64</v>
       </c>
@@ -3868,12 +2887,8 @@
       <c r="G66" s="1">
         <v>70</v>
       </c>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
-      <c r="K66" s="2"/>
-    </row>
-    <row r="67" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>65</v>
       </c>
@@ -3895,12 +2910,8 @@
       <c r="G67" s="1">
         <v>71</v>
       </c>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
-    </row>
-    <row r="68" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>66</v>
       </c>
@@ -3922,12 +2933,8 @@
       <c r="G68" s="1">
         <v>72</v>
       </c>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
-      <c r="K68" s="2"/>
-    </row>
-    <row r="69" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>67</v>
       </c>
@@ -3949,12 +2956,8 @@
       <c r="G69" s="1">
         <v>73</v>
       </c>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
-      <c r="K69" s="2"/>
-    </row>
-    <row r="70" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>68</v>
       </c>
@@ -3976,12 +2979,8 @@
       <c r="G70" s="1">
         <v>74</v>
       </c>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
-      <c r="K70" s="2"/>
-    </row>
-    <row r="71" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>69</v>
       </c>
@@ -4003,12 +3002,8 @@
       <c r="G71" s="1">
         <v>75</v>
       </c>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
-      <c r="J71" s="2"/>
-      <c r="K71" s="2"/>
-    </row>
-    <row r="72" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>70</v>
       </c>
@@ -4030,12 +3025,8 @@
       <c r="G72" s="1">
         <v>76</v>
       </c>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
-      <c r="J72" s="2"/>
-      <c r="K72" s="2"/>
-    </row>
-    <row r="73" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>71</v>
       </c>
@@ -4057,12 +3048,8 @@
       <c r="G73" s="1">
         <v>77</v>
       </c>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="K73" s="2"/>
-    </row>
-    <row r="74" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>72</v>
       </c>
@@ -4084,12 +3071,8 @@
       <c r="G74" s="1">
         <v>78</v>
       </c>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
-      <c r="J74" s="2"/>
-      <c r="K74" s="2"/>
-    </row>
-    <row r="75" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>73</v>
       </c>
@@ -4111,12 +3094,8 @@
       <c r="G75" s="1">
         <v>79</v>
       </c>
-      <c r="H75" s="2"/>
-      <c r="I75" s="2"/>
-      <c r="J75" s="2"/>
-      <c r="K75" s="2"/>
-    </row>
-    <row r="76" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="76" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>74</v>
       </c>
@@ -4138,12 +3117,8 @@
       <c r="G76" s="1">
         <v>80</v>
       </c>
-      <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
-      <c r="K76" s="2"/>
-    </row>
-    <row r="77" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>75</v>
       </c>
@@ -4165,12 +3140,8 @@
       <c r="G77" s="1">
         <v>81</v>
       </c>
-      <c r="H77" s="2"/>
-      <c r="I77" s="2"/>
-      <c r="J77" s="2"/>
-      <c r="K77" s="2"/>
-    </row>
-    <row r="78" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>76</v>
       </c>
@@ -4192,12 +3163,8 @@
       <c r="G78" s="1">
         <v>83</v>
       </c>
-      <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
-      <c r="K78" s="2"/>
-    </row>
-    <row r="79" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="79" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>77</v>
       </c>
@@ -4219,12 +3186,8 @@
       <c r="G79" s="1">
         <v>84</v>
       </c>
-      <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
-      <c r="J79" s="2"/>
-      <c r="K79" s="2"/>
-    </row>
-    <row r="80" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="80" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>78</v>
       </c>
@@ -4246,12 +3209,8 @@
       <c r="G80" s="1">
         <v>85</v>
       </c>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
-      <c r="J80" s="2"/>
-      <c r="K80" s="2"/>
-    </row>
-    <row r="81" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="81" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>79</v>
       </c>
@@ -4273,12 +3232,8 @@
       <c r="G81" s="1">
         <v>86</v>
       </c>
-      <c r="H81" s="2"/>
-      <c r="I81" s="2"/>
-      <c r="J81" s="2"/>
-      <c r="K81" s="2"/>
-    </row>
-    <row r="82" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="82" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>80</v>
       </c>
@@ -4300,12 +3255,8 @@
       <c r="G82" s="1">
         <v>87</v>
       </c>
-      <c r="H82" s="2"/>
-      <c r="I82" s="2"/>
-      <c r="J82" s="2"/>
-      <c r="K82" s="2"/>
-    </row>
-    <row r="83" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="83" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>81</v>
       </c>
@@ -4327,12 +3278,8 @@
       <c r="G83" s="1">
         <v>88</v>
       </c>
-      <c r="H83" s="2"/>
-      <c r="I83" s="2"/>
-      <c r="J83" s="2"/>
-      <c r="K83" s="2"/>
-    </row>
-    <row r="84" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>82</v>
       </c>
@@ -4354,12 +3301,8 @@
       <c r="G84" s="1">
         <v>89</v>
       </c>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2"/>
-      <c r="J84" s="2"/>
-      <c r="K84" s="2"/>
-    </row>
-    <row r="85" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="85" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>83</v>
       </c>
@@ -4381,12 +3324,8 @@
       <c r="G85" s="1">
         <v>90</v>
       </c>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="2"/>
-      <c r="K85" s="2"/>
-    </row>
-    <row r="86" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="86" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>84</v>
       </c>
@@ -4408,12 +3347,8 @@
       <c r="G86" s="1">
         <v>91</v>
       </c>
-      <c r="H86" s="2"/>
-      <c r="I86" s="2"/>
-      <c r="J86" s="2"/>
-      <c r="K86" s="2"/>
-    </row>
-    <row r="87" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>85</v>
       </c>
@@ -4435,12 +3370,8 @@
       <c r="G87" s="1">
         <v>92</v>
       </c>
-      <c r="H87" s="2"/>
-      <c r="I87" s="2"/>
-      <c r="J87" s="2"/>
-      <c r="K87" s="2"/>
-    </row>
-    <row r="88" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="88" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>86</v>
       </c>
@@ -4462,12 +3393,8 @@
       <c r="G88" s="1">
         <v>93</v>
       </c>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
-      <c r="J88" s="2"/>
-      <c r="K88" s="2"/>
-    </row>
-    <row r="89" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>87</v>
       </c>
@@ -4489,12 +3416,8 @@
       <c r="G89" s="1">
         <v>94</v>
       </c>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
-      <c r="K89" s="2"/>
-    </row>
-    <row r="90" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="90" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>88</v>
       </c>
@@ -4516,12 +3439,8 @@
       <c r="G90" s="1">
         <v>96</v>
       </c>
-      <c r="H90" s="2"/>
-      <c r="I90" s="2"/>
-      <c r="J90" s="2"/>
-      <c r="K90" s="2"/>
-    </row>
-    <row r="91" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>89</v>
       </c>
@@ -4543,12 +3462,8 @@
       <c r="G91" s="1">
         <v>97</v>
       </c>
-      <c r="H91" s="2"/>
-      <c r="I91" s="2"/>
-      <c r="J91" s="2"/>
-      <c r="K91" s="2"/>
-    </row>
-    <row r="92" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="92" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>90</v>
       </c>
@@ -4570,12 +3485,8 @@
       <c r="G92" s="1">
         <v>98</v>
       </c>
-      <c r="H92" s="2"/>
-      <c r="I92" s="2"/>
-      <c r="J92" s="2"/>
-      <c r="K92" s="2"/>
-    </row>
-    <row r="93" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="93" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>91</v>
       </c>
@@ -4597,12 +3508,8 @@
       <c r="G93" s="1">
         <v>99</v>
       </c>
-      <c r="H93" s="2"/>
-      <c r="I93" s="2"/>
-      <c r="J93" s="2"/>
-      <c r="K93" s="2"/>
-    </row>
-    <row r="94" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="94" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>92</v>
       </c>
@@ -4624,12 +3531,8 @@
       <c r="G94" s="1">
         <v>100</v>
       </c>
-      <c r="H94" s="2"/>
-      <c r="I94" s="2"/>
-      <c r="J94" s="2"/>
-      <c r="K94" s="2"/>
-    </row>
-    <row r="95" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="95" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>93</v>
       </c>
@@ -4651,12 +3554,8 @@
       <c r="G95" s="1">
         <v>101</v>
       </c>
-      <c r="H95" s="2"/>
-      <c r="I95" s="2"/>
-      <c r="J95" s="2"/>
-      <c r="K95" s="2"/>
-    </row>
-    <row r="96" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="96" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>94</v>
       </c>
@@ -4678,12 +3577,8 @@
       <c r="G96" s="1">
         <v>102</v>
       </c>
-      <c r="H96" s="2"/>
-      <c r="I96" s="2"/>
-      <c r="J96" s="2"/>
-      <c r="K96" s="2"/>
-    </row>
-    <row r="97" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="97" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>95</v>
       </c>
@@ -4705,12 +3600,8 @@
       <c r="G97" s="1">
         <v>103</v>
       </c>
-      <c r="H97" s="2"/>
-      <c r="I97" s="2"/>
-      <c r="J97" s="2"/>
-      <c r="K97" s="2"/>
-    </row>
-    <row r="98" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
         <v>96</v>
       </c>
@@ -4732,12 +3623,8 @@
       <c r="G98" s="1">
         <v>104</v>
       </c>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
-      <c r="J98" s="2"/>
-      <c r="K98" s="2"/>
-    </row>
-    <row r="99" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="99" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>97</v>
       </c>
@@ -4759,12 +3646,8 @@
       <c r="G99" s="1">
         <v>105</v>
       </c>
-      <c r="H99" s="2"/>
-      <c r="I99" s="2"/>
-      <c r="J99" s="2"/>
-      <c r="K99" s="2"/>
-    </row>
-    <row r="100" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="100" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>98</v>
       </c>
@@ -4786,12 +3669,8 @@
       <c r="G100" s="1">
         <v>106</v>
       </c>
-      <c r="H100" s="2"/>
-      <c r="I100" s="2"/>
-      <c r="J100" s="2"/>
-      <c r="K100" s="2"/>
-    </row>
-    <row r="101" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="101" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
         <v>99</v>
       </c>
@@ -4813,12 +3692,8 @@
       <c r="G101" s="1">
         <v>107</v>
       </c>
-      <c r="H101" s="2"/>
-      <c r="I101" s="2"/>
-      <c r="J101" s="2"/>
-      <c r="K101" s="2"/>
-    </row>
-    <row r="102" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="102" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
         <v>100</v>
       </c>
@@ -4840,12 +3715,8 @@
       <c r="G102" s="1">
         <v>108</v>
       </c>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
-      <c r="J102" s="2"/>
-      <c r="K102" s="2"/>
-    </row>
-    <row r="103" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="103" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>101</v>
       </c>
@@ -4867,12 +3738,8 @@
       <c r="G103" s="1">
         <v>109</v>
       </c>
-      <c r="H103" s="2"/>
-      <c r="I103" s="2"/>
-      <c r="J103" s="2"/>
-      <c r="K103" s="2"/>
-    </row>
-    <row r="104" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>102</v>
       </c>
@@ -4894,12 +3761,8 @@
       <c r="G104" s="1">
         <v>110</v>
       </c>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
-      <c r="J104" s="2"/>
-      <c r="K104" s="2"/>
-    </row>
-    <row r="105" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="105" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
         <v>103</v>
       </c>
@@ -4921,12 +3784,8 @@
       <c r="G105" s="1">
         <v>111</v>
       </c>
-      <c r="H105" s="2"/>
-      <c r="I105" s="2"/>
-      <c r="J105" s="2"/>
-      <c r="K105" s="2"/>
-    </row>
-    <row r="106" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="106" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>104</v>
       </c>
@@ -4948,12 +3807,8 @@
       <c r="G106" s="1">
         <v>112</v>
       </c>
-      <c r="H106" s="2"/>
-      <c r="I106" s="2"/>
-      <c r="J106" s="2"/>
-      <c r="K106" s="2"/>
-    </row>
-    <row r="107" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="107" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
         <v>105</v>
       </c>
@@ -4975,12 +3830,8 @@
       <c r="G107" s="1">
         <v>113</v>
       </c>
-      <c r="H107" s="2"/>
-      <c r="I107" s="2"/>
-      <c r="J107" s="2"/>
-      <c r="K107" s="2"/>
-    </row>
-    <row r="108" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="108" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>106</v>
       </c>
@@ -5002,12 +3853,8 @@
       <c r="G108" s="1">
         <v>114</v>
       </c>
-      <c r="H108" s="2"/>
-      <c r="I108" s="2"/>
-      <c r="J108" s="2"/>
-      <c r="K108" s="2"/>
-    </row>
-    <row r="109" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="109" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
         <v>107</v>
       </c>
@@ -5029,12 +3876,8 @@
       <c r="G109" s="1">
         <v>115</v>
       </c>
-      <c r="H109" s="2"/>
-      <c r="I109" s="2"/>
-      <c r="J109" s="2"/>
-      <c r="K109" s="2"/>
-    </row>
-    <row r="110" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="110" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>108</v>
       </c>
@@ -5056,12 +3899,8 @@
       <c r="G110" s="1">
         <v>116</v>
       </c>
-      <c r="H110" s="2"/>
-      <c r="I110" s="2"/>
-      <c r="J110" s="2"/>
-      <c r="K110" s="2"/>
-    </row>
-    <row r="111" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="111" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>109</v>
       </c>
@@ -5083,12 +3922,8 @@
       <c r="G111" s="1">
         <v>117</v>
       </c>
-      <c r="H111" s="2"/>
-      <c r="I111" s="2"/>
-      <c r="J111" s="2"/>
-      <c r="K111" s="2"/>
-    </row>
-    <row r="112" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="112" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
         <v>110</v>
       </c>
@@ -5110,12 +3945,8 @@
       <c r="G112" s="1">
         <v>118</v>
       </c>
-      <c r="H112" s="2"/>
-      <c r="I112" s="2"/>
-      <c r="J112" s="2"/>
-      <c r="K112" s="2"/>
-    </row>
-    <row r="113" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="113" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
         <v>111</v>
       </c>
@@ -5137,12 +3968,8 @@
       <c r="G113" s="1">
         <v>119</v>
       </c>
-      <c r="H113" s="2"/>
-      <c r="I113" s="2"/>
-      <c r="J113" s="2"/>
-      <c r="K113" s="2"/>
-    </row>
-    <row r="114" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="114" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
         <v>112</v>
       </c>
@@ -5164,12 +3991,8 @@
       <c r="G114" s="1">
         <v>120</v>
       </c>
-      <c r="H114" s="2"/>
-      <c r="I114" s="2"/>
-      <c r="J114" s="2"/>
-      <c r="K114" s="2"/>
-    </row>
-    <row r="115" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="115" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
         <v>113</v>
       </c>
@@ -5191,12 +4014,8 @@
       <c r="G115" s="1">
         <v>121</v>
       </c>
-      <c r="H115" s="2"/>
-      <c r="I115" s="2"/>
-      <c r="J115" s="2"/>
-      <c r="K115" s="2"/>
-    </row>
-    <row r="116" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="116" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="3">
         <v>114</v>
       </c>
@@ -5218,12 +4037,8 @@
       <c r="G116" s="1">
         <v>122</v>
       </c>
-      <c r="H116" s="2"/>
-      <c r="I116" s="2"/>
-      <c r="J116" s="2"/>
-      <c r="K116" s="2"/>
-    </row>
-    <row r="117" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="117" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="3">
         <v>115</v>
       </c>
@@ -5245,12 +4060,8 @@
       <c r="G117" s="1">
         <v>123</v>
       </c>
-      <c r="H117" s="2"/>
-      <c r="I117" s="2"/>
-      <c r="J117" s="2"/>
-      <c r="K117" s="2"/>
-    </row>
-    <row r="118" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="118" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="3">
         <v>116</v>
       </c>
@@ -5272,12 +4083,8 @@
       <c r="G118" s="1">
         <v>124</v>
       </c>
-      <c r="H118" s="2"/>
-      <c r="I118" s="2"/>
-      <c r="J118" s="2"/>
-      <c r="K118" s="2"/>
-    </row>
-    <row r="119" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="119" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
         <v>117</v>
       </c>
@@ -5299,12 +4106,8 @@
       <c r="G119" s="1">
         <v>125</v>
       </c>
-      <c r="H119" s="2"/>
-      <c r="I119" s="2"/>
-      <c r="J119" s="2"/>
-      <c r="K119" s="2"/>
-    </row>
-    <row r="120" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="120" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="3">
         <v>118</v>
       </c>
@@ -5326,12 +4129,8 @@
       <c r="G120" s="1">
         <v>127</v>
       </c>
-      <c r="H120" s="2"/>
-      <c r="I120" s="2"/>
-      <c r="J120" s="2"/>
-      <c r="K120" s="2"/>
-    </row>
-    <row r="121" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="121" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="3">
         <v>119</v>
       </c>
@@ -5353,12 +4152,8 @@
       <c r="G121" s="1">
         <v>128</v>
       </c>
-      <c r="H121" s="2"/>
-      <c r="I121" s="2"/>
-      <c r="J121" s="2"/>
-      <c r="K121" s="2"/>
-    </row>
-    <row r="122" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="122" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="3">
         <v>120</v>
       </c>
@@ -5380,12 +4175,8 @@
       <c r="G122" s="1">
         <v>129</v>
       </c>
-      <c r="H122" s="2"/>
-      <c r="I122" s="2"/>
-      <c r="J122" s="2"/>
-      <c r="K122" s="2"/>
-    </row>
-    <row r="123" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="123" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="3">
         <v>121</v>
       </c>
@@ -5407,12 +4198,8 @@
       <c r="G123" s="1">
         <v>130</v>
       </c>
-      <c r="H123" s="2"/>
-      <c r="I123" s="2"/>
-      <c r="J123" s="2"/>
-      <c r="K123" s="2"/>
-    </row>
-    <row r="124" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="124" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
         <v>122</v>
       </c>
@@ -5434,12 +4221,8 @@
       <c r="G124" s="1">
         <v>131</v>
       </c>
-      <c r="H124" s="2"/>
-      <c r="I124" s="2"/>
-      <c r="J124" s="2"/>
-      <c r="K124" s="2"/>
-    </row>
-    <row r="125" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="125" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="3">
         <v>123</v>
       </c>
@@ -5461,12 +4244,8 @@
       <c r="G125" s="1">
         <v>132</v>
       </c>
-      <c r="H125" s="2"/>
-      <c r="I125" s="2"/>
-      <c r="J125" s="2"/>
-      <c r="K125" s="2"/>
-    </row>
-    <row r="126" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="126" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
         <v>124</v>
       </c>
@@ -5488,12 +4267,8 @@
       <c r="G126" s="1">
         <v>133</v>
       </c>
-      <c r="H126" s="2"/>
-      <c r="I126" s="2"/>
-      <c r="J126" s="2"/>
-      <c r="K126" s="2"/>
-    </row>
-    <row r="127" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="127" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="3">
         <v>125</v>
       </c>
@@ -5515,12 +4290,8 @@
       <c r="G127" s="1">
         <v>134</v>
       </c>
-      <c r="H127" s="2"/>
-      <c r="I127" s="2"/>
-      <c r="J127" s="2"/>
-      <c r="K127" s="2"/>
-    </row>
-    <row r="128" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="128" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="3">
         <v>126</v>
       </c>
@@ -5542,12 +4313,8 @@
       <c r="G128" s="1">
         <v>135</v>
       </c>
-      <c r="H128" s="2"/>
-      <c r="I128" s="2"/>
-      <c r="J128" s="2"/>
-      <c r="K128" s="2"/>
-    </row>
-    <row r="129" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="129" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
         <v>127</v>
       </c>
@@ -5569,12 +4336,8 @@
       <c r="G129" s="1">
         <v>136</v>
       </c>
-      <c r="H129" s="2"/>
-      <c r="I129" s="2"/>
-      <c r="J129" s="2"/>
-      <c r="K129" s="2"/>
-    </row>
-    <row r="130" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="130" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="3">
         <v>128</v>
       </c>
@@ -5596,12 +4359,8 @@
       <c r="G130" s="1">
         <v>137</v>
       </c>
-      <c r="H130" s="2"/>
-      <c r="I130" s="2"/>
-      <c r="J130" s="2"/>
-      <c r="K130" s="2"/>
-    </row>
-    <row r="131" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="131" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="3">
         <v>129</v>
       </c>
@@ -5623,12 +4382,8 @@
       <c r="G131" s="1">
         <v>138</v>
       </c>
-      <c r="H131" s="2"/>
-      <c r="I131" s="2"/>
-      <c r="J131" s="2"/>
-      <c r="K131" s="2"/>
-    </row>
-    <row r="132" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="132" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="3">
         <v>130</v>
       </c>
@@ -5650,12 +4405,8 @@
       <c r="G132" s="1">
         <v>139</v>
       </c>
-      <c r="H132" s="2"/>
-      <c r="I132" s="2"/>
-      <c r="J132" s="2"/>
-      <c r="K132" s="2"/>
-    </row>
-    <row r="133" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="133" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="3">
         <v>131</v>
       </c>
@@ -5677,12 +4428,8 @@
       <c r="G133" s="1">
         <v>140</v>
       </c>
-      <c r="H133" s="2"/>
-      <c r="I133" s="2"/>
-      <c r="J133" s="2"/>
-      <c r="K133" s="2"/>
-    </row>
-    <row r="134" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="134" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="3">
         <v>132</v>
       </c>
@@ -5704,12 +4451,8 @@
       <c r="G134" s="1">
         <v>141</v>
       </c>
-      <c r="H134" s="2"/>
-      <c r="I134" s="2"/>
-      <c r="J134" s="2"/>
-      <c r="K134" s="2"/>
-    </row>
-    <row r="135" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="135" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="3">
         <v>133</v>
       </c>
@@ -5731,12 +4474,8 @@
       <c r="G135" s="1">
         <v>142</v>
       </c>
-      <c r="H135" s="2"/>
-      <c r="I135" s="2"/>
-      <c r="J135" s="2"/>
-      <c r="K135" s="2"/>
-    </row>
-    <row r="136" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="136" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="3">
         <v>134</v>
       </c>
@@ -5758,12 +4497,8 @@
       <c r="G136" s="1">
         <v>143</v>
       </c>
-      <c r="H136" s="2"/>
-      <c r="I136" s="2"/>
-      <c r="J136" s="2"/>
-      <c r="K136" s="2"/>
-    </row>
-    <row r="137" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="137" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="3">
         <v>135</v>
       </c>
@@ -5785,12 +4520,8 @@
       <c r="G137" s="1">
         <v>144</v>
       </c>
-      <c r="H137" s="2"/>
-      <c r="I137" s="2"/>
-      <c r="J137" s="2"/>
-      <c r="K137" s="2"/>
-    </row>
-    <row r="138" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="138" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="3">
         <v>136</v>
       </c>
@@ -5812,12 +4543,8 @@
       <c r="G138" s="1">
         <v>145</v>
       </c>
-      <c r="H138" s="2"/>
-      <c r="I138" s="2"/>
-      <c r="J138" s="2"/>
-      <c r="K138" s="2"/>
-    </row>
-    <row r="139" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="139" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="3">
         <v>137</v>
       </c>
@@ -5839,12 +4566,8 @@
       <c r="G139" s="1">
         <v>146</v>
       </c>
-      <c r="H139" s="2"/>
-      <c r="I139" s="2"/>
-      <c r="J139" s="2"/>
-      <c r="K139" s="2"/>
-    </row>
-    <row r="140" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="140" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="3">
         <v>138</v>
       </c>
@@ -5866,12 +4589,8 @@
       <c r="G140" s="1">
         <v>147</v>
       </c>
-      <c r="H140" s="2"/>
-      <c r="I140" s="2"/>
-      <c r="J140" s="2"/>
-      <c r="K140" s="2"/>
-    </row>
-    <row r="141" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="141" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="3">
         <v>139</v>
       </c>
@@ -5893,12 +4612,8 @@
       <c r="G141" s="1">
         <v>148</v>
       </c>
-      <c r="H141" s="2"/>
-      <c r="I141" s="2"/>
-      <c r="J141" s="2"/>
-      <c r="K141" s="2"/>
-    </row>
-    <row r="142" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="142" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="3">
         <v>140</v>
       </c>
@@ -5920,12 +4635,8 @@
       <c r="G142" s="1">
         <v>149</v>
       </c>
-      <c r="H142" s="2"/>
-      <c r="I142" s="2"/>
-      <c r="J142" s="2"/>
-      <c r="K142" s="2"/>
-    </row>
-    <row r="143" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="143" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="3">
         <v>141</v>
       </c>
@@ -5947,12 +4658,8 @@
       <c r="G143" s="1">
         <v>150</v>
       </c>
-      <c r="H143" s="2"/>
-      <c r="I143" s="2"/>
-      <c r="J143" s="2"/>
-      <c r="K143" s="2"/>
-    </row>
-    <row r="144" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="144" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="3">
         <v>142</v>
       </c>
@@ -5974,12 +4681,8 @@
       <c r="G144" s="1">
         <v>151</v>
       </c>
-      <c r="H144" s="2"/>
-      <c r="I144" s="2"/>
-      <c r="J144" s="2"/>
-      <c r="K144" s="2"/>
-    </row>
-    <row r="145" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="145" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" s="3">
         <v>143</v>
       </c>
@@ -6001,12 +4704,8 @@
       <c r="G145" s="1">
         <v>152</v>
       </c>
-      <c r="H145" s="2"/>
-      <c r="I145" s="2"/>
-      <c r="J145" s="2"/>
-      <c r="K145" s="2"/>
-    </row>
-    <row r="146" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="146" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" s="3">
         <v>144</v>
       </c>
@@ -6028,12 +4727,8 @@
       <c r="G146" s="1">
         <v>153</v>
       </c>
-      <c r="H146" s="2"/>
-      <c r="I146" s="2"/>
-      <c r="J146" s="2"/>
-      <c r="K146" s="2"/>
-    </row>
-    <row r="147" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="147" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="3">
         <v>145</v>
       </c>
@@ -6055,12 +4750,8 @@
       <c r="G147" s="1">
         <v>154</v>
       </c>
-      <c r="H147" s="2"/>
-      <c r="I147" s="2"/>
-      <c r="J147" s="2"/>
-      <c r="K147" s="2"/>
-    </row>
-    <row r="148" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="148" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="3">
         <v>146</v>
       </c>
@@ -6082,12 +4773,8 @@
       <c r="G148" s="1">
         <v>155</v>
       </c>
-      <c r="H148" s="2"/>
-      <c r="I148" s="2"/>
-      <c r="J148" s="2"/>
-      <c r="K148" s="2"/>
-    </row>
-    <row r="149" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="149" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="3">
         <v>147</v>
       </c>
@@ -6109,12 +4796,8 @@
       <c r="G149" s="1">
         <v>156</v>
       </c>
-      <c r="H149" s="2"/>
-      <c r="I149" s="2"/>
-      <c r="J149" s="2"/>
-      <c r="K149" s="2"/>
-    </row>
-    <row r="150" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="150" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="3">
         <v>148</v>
       </c>
@@ -6136,12 +4819,8 @@
       <c r="G150" s="1">
         <v>157</v>
       </c>
-      <c r="H150" s="2"/>
-      <c r="I150" s="2"/>
-      <c r="J150" s="2"/>
-      <c r="K150" s="2"/>
-    </row>
-    <row r="151" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="151" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="3">
         <v>149</v>
       </c>
@@ -6163,12 +4842,8 @@
       <c r="G151" s="1">
         <v>158</v>
       </c>
-      <c r="H151" s="2"/>
-      <c r="I151" s="2"/>
-      <c r="J151" s="2"/>
-      <c r="K151" s="2"/>
-    </row>
-    <row r="152" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="152" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="3">
         <v>150</v>
       </c>
@@ -6190,12 +4865,8 @@
       <c r="G152" s="1">
         <v>159</v>
       </c>
-      <c r="H152" s="2"/>
-      <c r="I152" s="2"/>
-      <c r="J152" s="2"/>
-      <c r="K152" s="2"/>
-    </row>
-    <row r="153" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="153" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" s="3">
         <v>151</v>
       </c>
@@ -6217,12 +4888,8 @@
       <c r="G153" s="1">
         <v>160</v>
       </c>
-      <c r="H153" s="2"/>
-      <c r="I153" s="2"/>
-      <c r="J153" s="2"/>
-      <c r="K153" s="2"/>
-    </row>
-    <row r="154" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="154" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="3">
         <v>152</v>
       </c>
@@ -6244,12 +4911,8 @@
       <c r="G154" s="1">
         <v>161</v>
       </c>
-      <c r="H154" s="2"/>
-      <c r="I154" s="2"/>
-      <c r="J154" s="2"/>
-      <c r="K154" s="2"/>
-    </row>
-    <row r="155" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="155" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" s="3">
         <v>153</v>
       </c>
@@ -6271,12 +4934,8 @@
       <c r="G155" s="1">
         <v>162</v>
       </c>
-      <c r="H155" s="2"/>
-      <c r="I155" s="2"/>
-      <c r="J155" s="2"/>
-      <c r="K155" s="2"/>
-    </row>
-    <row r="156" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="156" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="3">
         <v>154</v>
       </c>
@@ -6298,12 +4957,8 @@
       <c r="G156" s="1">
         <v>163</v>
       </c>
-      <c r="H156" s="2"/>
-      <c r="I156" s="2"/>
-      <c r="J156" s="2"/>
-      <c r="K156" s="2"/>
-    </row>
-    <row r="157" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="157" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="3">
         <v>155</v>
       </c>
@@ -6325,12 +4980,8 @@
       <c r="G157" s="1">
         <v>164</v>
       </c>
-      <c r="H157" s="2"/>
-      <c r="I157" s="2"/>
-      <c r="J157" s="2"/>
-      <c r="K157" s="2"/>
-    </row>
-    <row r="158" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="158" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="3">
         <v>156</v>
       </c>
@@ -6352,12 +5003,8 @@
       <c r="G158" s="1">
         <v>165</v>
       </c>
-      <c r="H158" s="2"/>
-      <c r="I158" s="2"/>
-      <c r="J158" s="2"/>
-      <c r="K158" s="2"/>
-    </row>
-    <row r="159" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="159" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="3">
         <v>157</v>
       </c>
@@ -6379,12 +5026,8 @@
       <c r="G159" s="1">
         <v>166</v>
       </c>
-      <c r="H159" s="2"/>
-      <c r="I159" s="2"/>
-      <c r="J159" s="2"/>
-      <c r="K159" s="2"/>
-    </row>
-    <row r="160" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="160" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="3">
         <v>158</v>
       </c>
@@ -6406,12 +5049,8 @@
       <c r="G160" s="1">
         <v>167</v>
       </c>
-      <c r="H160" s="2"/>
-      <c r="I160" s="2"/>
-      <c r="J160" s="2"/>
-      <c r="K160" s="2"/>
-    </row>
-    <row r="161" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="161" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="3">
         <v>159</v>
       </c>
@@ -6433,12 +5072,8 @@
       <c r="G161" s="1">
         <v>168</v>
       </c>
-      <c r="H161" s="2"/>
-      <c r="I161" s="2"/>
-      <c r="J161" s="2"/>
-      <c r="K161" s="2"/>
-    </row>
-    <row r="162" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="162" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="3">
         <v>160</v>
       </c>
@@ -6460,12 +5095,8 @@
       <c r="G162" s="1">
         <v>169</v>
       </c>
-      <c r="H162" s="2"/>
-      <c r="I162" s="2"/>
-      <c r="J162" s="2"/>
-      <c r="K162" s="2"/>
-    </row>
-    <row r="163" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="163" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="3">
         <v>161</v>
       </c>
@@ -6487,12 +5118,8 @@
       <c r="G163" s="1">
         <v>170</v>
       </c>
-      <c r="H163" s="2"/>
-      <c r="I163" s="2"/>
-      <c r="J163" s="2"/>
-      <c r="K163" s="2"/>
-    </row>
-    <row r="164" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="164" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" s="3">
         <v>162</v>
       </c>
@@ -6514,12 +5141,8 @@
       <c r="G164" s="1">
         <v>171</v>
       </c>
-      <c r="H164" s="2"/>
-      <c r="I164" s="2"/>
-      <c r="J164" s="2"/>
-      <c r="K164" s="2"/>
-    </row>
-    <row r="165" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="165" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="3">
         <v>163</v>
       </c>
@@ -6541,12 +5164,8 @@
       <c r="G165" s="1">
         <v>172</v>
       </c>
-      <c r="H165" s="2"/>
-      <c r="I165" s="2"/>
-      <c r="J165" s="2"/>
-      <c r="K165" s="2"/>
-    </row>
-    <row r="166" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="166" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="3">
         <v>164</v>
       </c>
@@ -6568,12 +5187,8 @@
       <c r="G166" s="1">
         <v>173</v>
       </c>
-      <c r="H166" s="2"/>
-      <c r="I166" s="2"/>
-      <c r="J166" s="2"/>
-      <c r="K166" s="2"/>
-    </row>
-    <row r="167" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="167" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="3">
         <v>165</v>
       </c>
@@ -6595,12 +5210,8 @@
       <c r="G167" s="1">
         <v>174</v>
       </c>
-      <c r="H167" s="2"/>
-      <c r="I167" s="2"/>
-      <c r="J167" s="2"/>
-      <c r="K167" s="2"/>
-    </row>
-    <row r="168" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="168" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" s="3">
         <v>166</v>
       </c>
@@ -6622,12 +5233,8 @@
       <c r="G168" s="1">
         <v>175</v>
       </c>
-      <c r="H168" s="2"/>
-      <c r="I168" s="2"/>
-      <c r="J168" s="2"/>
-      <c r="K168" s="2"/>
-    </row>
-    <row r="169" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="169" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" s="3">
         <v>167</v>
       </c>
@@ -6649,12 +5256,8 @@
       <c r="G169" s="1">
         <v>176</v>
       </c>
-      <c r="H169" s="2"/>
-      <c r="I169" s="2"/>
-      <c r="J169" s="2"/>
-      <c r="K169" s="2"/>
-    </row>
-    <row r="170" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="170" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="3">
         <v>168</v>
       </c>
@@ -6676,12 +5279,8 @@
       <c r="G170" s="1">
         <v>177</v>
       </c>
-      <c r="H170" s="2"/>
-      <c r="I170" s="2"/>
-      <c r="J170" s="2"/>
-      <c r="K170" s="2"/>
-    </row>
-    <row r="171" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="171" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" s="3">
         <v>169</v>
       </c>
@@ -6703,12 +5302,8 @@
       <c r="G171" s="1">
         <v>178</v>
       </c>
-      <c r="H171" s="2"/>
-      <c r="I171" s="2"/>
-      <c r="J171" s="2"/>
-      <c r="K171" s="2"/>
-    </row>
-    <row r="172" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="172" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" s="3">
         <v>170</v>
       </c>
@@ -6730,12 +5325,8 @@
       <c r="G172" s="1">
         <v>179</v>
       </c>
-      <c r="H172" s="2"/>
-      <c r="I172" s="2"/>
-      <c r="J172" s="2"/>
-      <c r="K172" s="2"/>
-    </row>
-    <row r="173" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="173" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" s="3">
         <v>171</v>
       </c>
@@ -6757,12 +5348,8 @@
       <c r="G173" s="1">
         <v>180</v>
       </c>
-      <c r="H173" s="2"/>
-      <c r="I173" s="2"/>
-      <c r="J173" s="2"/>
-      <c r="K173" s="2"/>
-    </row>
-    <row r="174" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="174" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" s="3">
         <v>172</v>
       </c>
@@ -6784,12 +5371,8 @@
       <c r="G174" s="1">
         <v>181</v>
       </c>
-      <c r="H174" s="2"/>
-      <c r="I174" s="2"/>
-      <c r="J174" s="2"/>
-      <c r="K174" s="2"/>
-    </row>
-    <row r="175" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="175" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" s="3">
         <v>173</v>
       </c>
@@ -6811,12 +5394,8 @@
       <c r="G175" s="1">
         <v>182</v>
       </c>
-      <c r="H175" s="2"/>
-      <c r="I175" s="2"/>
-      <c r="J175" s="2"/>
-      <c r="K175" s="2"/>
-    </row>
-    <row r="176" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="176" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" s="3">
         <v>174</v>
       </c>
@@ -6838,12 +5417,8 @@
       <c r="G176" s="1">
         <v>183</v>
       </c>
-      <c r="H176" s="2"/>
-      <c r="I176" s="2"/>
-      <c r="J176" s="2"/>
-      <c r="K176" s="2"/>
-    </row>
-    <row r="177" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="177" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" s="3">
         <v>175</v>
       </c>
@@ -6865,12 +5440,8 @@
       <c r="G177" s="1">
         <v>184</v>
       </c>
-      <c r="H177" s="2"/>
-      <c r="I177" s="2"/>
-      <c r="J177" s="2"/>
-      <c r="K177" s="2"/>
-    </row>
-    <row r="178" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="178" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" s="3">
         <v>176</v>
       </c>
@@ -6892,12 +5463,8 @@
       <c r="G178" s="1">
         <v>185</v>
       </c>
-      <c r="H178" s="2"/>
-      <c r="I178" s="2"/>
-      <c r="J178" s="2"/>
-      <c r="K178" s="2"/>
-    </row>
-    <row r="179" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="179" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" s="3">
         <v>177</v>
       </c>
@@ -6919,12 +5486,8 @@
       <c r="G179" s="1">
         <v>186</v>
       </c>
-      <c r="H179" s="2"/>
-      <c r="I179" s="2"/>
-      <c r="J179" s="2"/>
-      <c r="K179" s="2"/>
-    </row>
-    <row r="180" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="180" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" s="3">
         <v>178</v>
       </c>
@@ -6946,12 +5509,8 @@
       <c r="G180" s="1">
         <v>187</v>
       </c>
-      <c r="H180" s="2"/>
-      <c r="I180" s="2"/>
-      <c r="J180" s="2"/>
-      <c r="K180" s="2"/>
-    </row>
-    <row r="181" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="181" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="3">
         <v>179</v>
       </c>
@@ -6973,12 +5532,8 @@
       <c r="G181" s="1">
         <v>188</v>
       </c>
-      <c r="H181" s="2"/>
-      <c r="I181" s="2"/>
-      <c r="J181" s="2"/>
-      <c r="K181" s="2"/>
-    </row>
-    <row r="182" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="182" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="3">
         <v>180</v>
       </c>
@@ -7000,12 +5555,8 @@
       <c r="G182" s="1">
         <v>189</v>
       </c>
-      <c r="H182" s="2"/>
-      <c r="I182" s="2"/>
-      <c r="J182" s="2"/>
-      <c r="K182" s="2"/>
-    </row>
-    <row r="183" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="183" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="3">
         <v>181</v>
       </c>
@@ -7027,12 +5578,8 @@
       <c r="G183" s="1">
         <v>190</v>
       </c>
-      <c r="H183" s="2"/>
-      <c r="I183" s="2"/>
-      <c r="J183" s="2"/>
-      <c r="K183" s="2"/>
-    </row>
-    <row r="184" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="184" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" s="3">
         <v>182</v>
       </c>
@@ -7054,12 +5601,8 @@
       <c r="G184" s="1">
         <v>192</v>
       </c>
-      <c r="H184" s="2"/>
-      <c r="I184" s="2"/>
-      <c r="J184" s="2"/>
-      <c r="K184" s="2"/>
-    </row>
-    <row r="185" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="185" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="3">
         <v>183</v>
       </c>
@@ -7081,12 +5624,8 @@
       <c r="G185" s="1">
         <v>193</v>
       </c>
-      <c r="H185" s="2"/>
-      <c r="I185" s="2"/>
-      <c r="J185" s="2"/>
-      <c r="K185" s="2"/>
-    </row>
-    <row r="186" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="186" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" s="3">
         <v>184</v>
       </c>
@@ -7108,12 +5647,8 @@
       <c r="G186" s="1">
         <v>194</v>
       </c>
-      <c r="H186" s="2"/>
-      <c r="I186" s="2"/>
-      <c r="J186" s="2"/>
-      <c r="K186" s="2"/>
-    </row>
-    <row r="187" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="187" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="3">
         <v>185</v>
       </c>
@@ -7135,12 +5670,8 @@
       <c r="G187" s="1">
         <v>195</v>
       </c>
-      <c r="H187" s="2"/>
-      <c r="I187" s="2"/>
-      <c r="J187" s="2"/>
-      <c r="K187" s="2"/>
-    </row>
-    <row r="188" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="188" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" s="3">
         <v>186</v>
       </c>
@@ -7162,12 +5693,8 @@
       <c r="G188" s="1">
         <v>196</v>
       </c>
-      <c r="H188" s="2"/>
-      <c r="I188" s="2"/>
-      <c r="J188" s="2"/>
-      <c r="K188" s="2"/>
-    </row>
-    <row r="189" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="189" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" s="3">
         <v>187</v>
       </c>
@@ -7189,12 +5716,8 @@
       <c r="G189" s="1">
         <v>197</v>
       </c>
-      <c r="H189" s="2"/>
-      <c r="I189" s="2"/>
-      <c r="J189" s="2"/>
-      <c r="K189" s="2"/>
-    </row>
-    <row r="190" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="190" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" s="3">
         <v>188</v>
       </c>
@@ -7216,12 +5739,8 @@
       <c r="G190" s="1">
         <v>198</v>
       </c>
-      <c r="H190" s="2"/>
-      <c r="I190" s="2"/>
-      <c r="J190" s="2"/>
-      <c r="K190" s="2"/>
-    </row>
-    <row r="191" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="191" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" s="3">
         <v>189</v>
       </c>
@@ -7243,12 +5762,8 @@
       <c r="G191" s="1">
         <v>199</v>
       </c>
-      <c r="H191" s="2"/>
-      <c r="I191" s="2"/>
-      <c r="J191" s="2"/>
-      <c r="K191" s="2"/>
-    </row>
-    <row r="192" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="192" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" s="3">
         <v>190</v>
       </c>
@@ -7270,18 +5785,13 @@
       <c r="G192" s="1">
         <v>200</v>
       </c>
-      <c r="H192" s="2"/>
-      <c r="I192" s="2"/>
-      <c r="J192" s="2"/>
-      <c r="K192" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="98" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>